<commit_message>
test results of algorithms
</commit_message>
<xml_diff>
--- a/game_records.xlsx
+++ b/game_records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-13 09:55:51</t>
+          <t>2025-05-13 12:18:01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A*</t>
+          <t>DFS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -478,35 +478,1401 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00:05.10</t>
+          <t>00:17.30</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>54</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-05-13 09:56:25</t>
+          <t>2025-05-13 12:19:14</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>00:17.30</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:20:14</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>00:17.30</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:21:01</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>A*</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Map 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>00:05.30</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E5" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:21:21</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:21:46</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:22:25</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>00:08.30</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:23:29</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>00:17.70</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:23:54</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>00:06.70</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:24:35</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>00:11.30</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:25:57</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>00:11.30</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:27:14</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>00:11.30</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:27:50</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>00:06.70</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:28:15</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>00:06.70</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:28:42</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>00:06.70</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:29:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:30:07</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:30:30</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:11:47</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>00:11.30</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:12:29</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>00:11.30</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:13:37</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>00:11.30</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:14:19</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:14:43</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:15:10</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:16:18</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>00:11.10</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:16:43</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>00:06.50</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:17:13</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>00:08.70</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:17:47</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:18:05</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:18:28</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:19:38</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>00:11.50</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:20:37</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>00:11.50</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:21:25</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>00:11.50</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:25:09</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:25:53</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:26:13</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Map 2</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:40:29</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:40:49</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:41:08</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>DFS</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:42:18</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:42:43</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:43:18</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:43:52</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:44:48</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>00:06.70</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:45:33</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>And-Or Search</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>00:10.10</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:46:14</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:46:33</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:46:51</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Steepest Ascent Hill Climbing</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-05-13 12:47:37</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>00:12.70</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:06:53</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>00:12.70</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:09:43</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Backtracking</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>00:12.70</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:10:15</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:10:35</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-05-13 13:10:53</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Q-Learning</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Map 3</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>00:04.50</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>72</v>
+      </c>
+      <c r="E57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-05-13 14:29:42</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-05-13 14:30:02</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>A*</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Map 1</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>00:05.30</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
         <v>54</v>
       </c>
     </row>

</xml_diff>